<commit_message>
update: get value of index of max rowcount
</commit_message>
<xml_diff>
--- a/spexcel_output.xlsx
+++ b/spexcel_output.xlsx
@@ -538,86 +538,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -628,59 +610,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -691,70 +664,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>